<commit_message>
Scripts e Modelagem Atualizados
</commit_message>
<xml_diff>
--- a/Modelagem Projeto Pedidos.xlsx
+++ b/Modelagem Projeto Pedidos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesher\Desktop\github Banco de Dados\Projeto_Pedidos em andamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3557685-0B15-4A57-9E83-7624343B7445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43AC66E-F1A3-4540-A137-C0FC6110BD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{9D68CBE9-E53A-4F1D-B8D6-B9437569FA67}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="74">
   <si>
     <t>Tipo</t>
   </si>
@@ -231,22 +231,22 @@
     <t>Cidades - Criada e Populada (3)</t>
   </si>
   <si>
-    <t>Itens_Pedidos (8)</t>
-  </si>
-  <si>
     <t>Codigo_Cidade_Cliente</t>
   </si>
   <si>
     <t>Produtos -  Criada e Populada (6)</t>
   </si>
   <si>
-    <t>Pedidos - Criada (7)</t>
-  </si>
-  <si>
     <t>Vendedores  - Criada e Populada (4)</t>
   </si>
   <si>
     <t>Clientes - Criada e Populada (5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pedidos - Criada (7) </t>
+  </si>
+  <si>
+    <t>Itens_Pedidos - Criada (8)</t>
   </si>
 </sst>
 </file>
@@ -299,7 +299,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,12 +309,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -446,13 +440,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -771,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8442C2FA-D554-4128-AF81-3E6B2310AF96}">
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:G30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +788,7 @@
     </row>
     <row r="2" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -922,7 +913,7 @@
     <row r="10" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="1:7" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
@@ -1033,7 +1024,7 @@
     </row>
     <row r="18" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>31</v>
@@ -1198,15 +1189,15 @@
     </row>
     <row r="29" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
+      <c r="A30" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
     </row>
     <row r="31" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
@@ -1354,15 +1345,15 @@
     <row r="40" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
+      <c r="A42" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
     </row>
     <row r="43" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
@@ -1395,9 +1386,7 @@
         <v>31</v>
       </c>
       <c r="C44" s="10"/>
-      <c r="D44" s="10" t="s">
-        <v>4</v>
-      </c>
+      <c r="D44" s="10"/>
       <c r="E44" s="10" t="s">
         <v>4</v>
       </c>
@@ -1501,15 +1490,15 @@
     <row r="51" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-      <c r="D53" s="21"/>
-      <c r="E53" s="21"/>
-      <c r="F53" s="21"/>
-      <c r="G53" s="21"/>
+      <c r="A53" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" s="19"/>
+      <c r="C53" s="19"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="19"/>
+      <c r="F53" s="19"/>
+      <c r="G53" s="19"/>
     </row>
     <row r="54" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
@@ -1612,15 +1601,15 @@
     <row r="60" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="63" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="21" t="s">
+      <c r="A63" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="21"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="21"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="19"/>
+      <c r="G63" s="19"/>
     </row>
     <row r="64" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
@@ -1710,15 +1699,15 @@
     <row r="69" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="21" t="s">
+      <c r="A72" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B72" s="21"/>
-      <c r="C72" s="21"/>
-      <c r="D72" s="21"/>
-      <c r="E72" s="21"/>
-      <c r="F72" s="21"/>
-      <c r="G72" s="21"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
     </row>
     <row r="73" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
@@ -1778,15 +1767,15 @@
     <row r="76" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="77" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="78" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="21" t="s">
+      <c r="A78" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B78" s="21"/>
-      <c r="C78" s="21"/>
-      <c r="D78" s="21"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="21"/>
-      <c r="G78" s="21"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="19"/>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="G78" s="19"/>
     </row>
     <row r="79" spans="1:7" ht="19.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
@@ -1875,18 +1864,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2034,18 +2023,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0C0EB2D-39AA-44E8-85DB-46139A0AE324}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5094A21-7D69-4413-8D6B-637D4F166F35}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B5094A21-7D69-4413-8D6B-637D4F166F35}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0C0EB2D-39AA-44E8-85DB-46139A0AE324}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>